<commit_message>
Small updates to Excel formatting.
</commit_message>
<xml_diff>
--- a/Excel/INFS 768 - Predictive Analytics/Quizzes/Quiz 1.xlsx
+++ b/Excel/INFS 768 - Predictive Analytics/Quizzes/Quiz 1.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25330"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ggobl\Dropbox\Dakota State University\Classes\INFS 768 Predictive Analytics\Quiz 1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ggobl\Documents\Portfolio\Excel\INFS 768 - Predictive Analytics\Quizzes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21EEA386-5FD6-4E14-BEE8-17446B961593}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D12759E4-28B0-4FA9-9CA6-D2BA84A0089E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -846,22 +846,6 @@
             </c:extLst>
           </c:dPt>
           <c:dLbls>
-            <c:dLbl>
-              <c:idx val="0"/>
-              <c:dLblPos val="t"/>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="1"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
-              <c:showBubbleSize val="0"/>
-              <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
-                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                  <c16:uniqueId val="{00000007-1B35-4DDD-BAA5-32D68BCBB1F5}"/>
-                </c:ext>
-              </c:extLst>
-            </c:dLbl>
             <c:spPr>
               <a:noFill/>
               <a:ln>
@@ -893,11 +877,12 @@
             </c:txPr>
             <c:dLblPos val="t"/>
             <c:showLegendKey val="0"/>
-            <c:showVal val="0"/>
+            <c:showVal val="1"/>
             <c:showCatName val="0"/>
             <c:showSerName val="0"/>
             <c:showPercent val="0"/>
             <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                 <c15:showLeaderLines val="1"/>
@@ -2327,7 +2312,7 @@
   <dimension ref="A1:G37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+      <selection activeCell="J17" sqref="J17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>

</xml_diff>

<commit_message>
Fixed a grammar error in Quiz 1 in Excel.
</commit_message>
<xml_diff>
--- a/Excel/INFS 768 - Predictive Analytics/Quizzes/Quiz 1.xlsx
+++ b/Excel/INFS 768 - Predictive Analytics/Quizzes/Quiz 1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ggobl\Documents\Portfolio\Excel\INFS 768 - Predictive Analytics\Quizzes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D12759E4-28B0-4FA9-9CA6-D2BA84A0089E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BB7095A-9193-4383-9CCA-42626425CDDB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -96,9 +96,14 @@
     <t>KNN Results for Unknown:</t>
   </si>
   <si>
+    <t>Answer to 
+discussion 
+Question</t>
+  </si>
+  <si>
     <r>
       <t xml:space="preserve">*Note on K=2: Used this quote from the scikit learn
-documentation to decide the value for this and decided the value based on distance.: "Warning Regarding the Nearest Neighbors algorithms, if two neighbors, neighbor k+1 and k, have identical distances but different labels, the results will depend on the ordering of the training data." </t>
+documentation to deduce the Default Status value based on distance.: "Warning Regarding the Nearest Neighbors algorithms, if two neighbors, neighbor k+1 and k, have identical distances but different labels, the results will depend on the ordering of the training data." </t>
     </r>
     <r>
       <rPr>
@@ -111,11 +116,6 @@
       </rPr>
       <t>source: https://scikit-learn.org/stable/modules/neighbors.html</t>
     </r>
-  </si>
-  <si>
-    <t>Answer to 
-discussion 
-Question</t>
   </si>
 </sst>
 </file>
@@ -2312,7 +2312,7 @@
   <dimension ref="A1:G37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J17" sqref="J17"/>
+      <selection activeCell="A22" sqref="A22:D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -2639,7 +2639,7 @@
         <v>13</v>
       </c>
       <c r="C14" s="16" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D14" s="17"/>
     </row>
@@ -2693,7 +2693,7 @@
     </row>
     <row r="22" spans="1:4" ht="130.19999999999999" customHeight="1">
       <c r="A22" s="15" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B22" s="15"/>
       <c r="C22" s="15"/>

</xml_diff>

<commit_message>
Small update to formatting of Excel quiz 1.
</commit_message>
<xml_diff>
--- a/Excel/INFS 768 - Predictive Analytics/Quizzes/Quiz 1.xlsx
+++ b/Excel/INFS 768 - Predictive Analytics/Quizzes/Quiz 1.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26227"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ggobl\Documents\Portfolio\Excel\INFS 768 - Predictive Analytics\Quizzes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BB7095A-9193-4383-9CCA-42626425CDDB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41FDF1BE-5211-42F3-8D84-4C32A15428D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -93,9 +93,6 @@
     <t>?</t>
   </si>
   <si>
-    <t>KNN Results for Unknown:</t>
-  </si>
-  <si>
     <t>Answer to 
 discussion 
 Question</t>
@@ -116,6 +113,10 @@
       </rPr>
       <t>source: https://scikit-learn.org/stable/modules/neighbors.html</t>
     </r>
+  </si>
+  <si>
+    <t>KNN Results for
+ Unknown:</t>
   </si>
 </sst>
 </file>
@@ -259,25 +260,25 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="44" fontId="3" fillId="3" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="44" fontId="3" fillId="3" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="44" fontId="3" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="3" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="44" fontId="3" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="44" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -290,17 +291,23 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="44" fontId="3" fillId="4" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="44" fontId="3" fillId="4" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="44" fontId="3" fillId="4" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="44" fontId="3" fillId="4" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2312,7 +2319,7 @@
   <dimension ref="A1:G37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A22" sqref="A22:D22"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -2635,11 +2642,12 @@
       </c>
     </row>
     <row r="14" spans="1:7" ht="50.4" customHeight="1">
-      <c r="A14" s="13" t="s">
+      <c r="A14" s="19" t="s">
+        <v>15</v>
+      </c>
+      <c r="B14" s="19"/>
+      <c r="C14" s="16" t="s">
         <v>13</v>
-      </c>
-      <c r="C14" s="16" t="s">
-        <v>14</v>
       </c>
       <c r="D14" s="17"/>
     </row>
@@ -2652,48 +2660,48 @@
       </c>
     </row>
     <row r="16" spans="1:7">
-      <c r="A16">
+      <c r="A16" s="18">
         <v>1</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B16" s="18" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="17" spans="1:4">
-      <c r="A17">
+      <c r="A17" s="18">
         <v>2</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B17" s="18" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="18" spans="1:4">
-      <c r="A18">
+      <c r="A18" s="18">
         <v>3</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B18" s="18" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="19" spans="1:4">
-      <c r="A19">
+      <c r="A19" s="18">
         <v>4</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B19" s="18" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="20" spans="1:4">
-      <c r="A20">
+      <c r="A20" s="18">
         <v>5</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B20" s="18" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="130.19999999999999" customHeight="1">
       <c r="A22" s="15" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B22" s="15"/>
       <c r="C22" s="15"/>
@@ -2707,9 +2715,10 @@
       <c r="A37" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="3">
     <mergeCell ref="A22:D22"/>
     <mergeCell ref="C14:D14"/>
+    <mergeCell ref="A14:B14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>